<commit_message>
modification écriture log pour export csv
adieu les virgules
</commit_message>
<xml_diff>
--- a/xp/log_questionnaire_XP_WEEK2_EXPLAINED.xlsx
+++ b/xp/log_questionnaire_XP_WEEK2_EXPLAINED.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1965" yWindow="0" windowWidth="27780" windowHeight="12285"/>
+    <workbookView xWindow="3855" yWindow="0" windowWidth="27780" windowHeight="12285"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="118">
   <si>
     <t>Questionnaire rewrite</t>
   </si>
@@ -375,13 +375,16 @@
   </si>
   <si>
     <t>IDjoueur</t>
+  </si>
+  <si>
+    <t>GLOBAL : transformer toutes les , en _</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,6 +403,14 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -502,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -574,6 +585,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -868,7 +882,7 @@
   <dimension ref="A1:E160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,6 +899,9 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="25" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -905,7 +922,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="26" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -918,7 +935,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
@@ -929,7 +946,7 @@
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
@@ -940,7 +957,7 @@
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
@@ -951,7 +968,7 @@
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="19" t="s">
         <v>10</v>
       </c>
@@ -962,7 +979,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="20"/>
       <c r="C9" s="6" t="s">
         <v>31</v>
@@ -973,7 +990,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="21"/>
       <c r="C10" s="11" t="s">
         <v>32</v>
@@ -984,7 +1001,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="9" t="s">
         <v>11</v>
       </c>
@@ -995,7 +1012,7 @@
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="9"/>
       <c r="C12" s="6" t="s">
         <v>29</v>
@@ -1006,7 +1023,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="9"/>
       <c r="C13" s="6" t="s">
         <v>30</v>
@@ -1017,7 +1034,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="22" t="s">
         <v>12</v>
       </c>
@@ -1028,7 +1045,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+      <c r="A15" s="27"/>
       <c r="B15" s="23"/>
       <c r="C15" s="6" t="s">
         <v>20</v>
@@ -1039,7 +1056,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="23"/>
       <c r="C16" s="6" t="s">
         <v>21</v>
@@ -1050,7 +1067,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="23"/>
       <c r="C17" s="6" t="s">
         <v>22</v>
@@ -1061,7 +1078,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="23"/>
       <c r="C18" s="6" t="s">
         <v>23</v>
@@ -1072,7 +1089,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="23"/>
       <c r="C19" s="6" t="s">
         <v>24</v>
@@ -1083,7 +1100,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="23"/>
       <c r="C20" s="6" t="s">
         <v>25</v>
@@ -1094,7 +1111,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="23"/>
       <c r="C21" s="6" t="s">
         <v>26</v>
@@ -1105,7 +1122,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="23"/>
       <c r="C22" s="6" t="s">
         <v>27</v>
@@ -1116,7 +1133,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="27"/>
+      <c r="A23" s="28"/>
       <c r="B23" s="24"/>
       <c r="C23" s="17" t="s">
         <v>28</v>
@@ -1127,7 +1144,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="26" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1140,7 +1157,7 @@
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
+      <c r="A25" s="27"/>
       <c r="B25" s="3"/>
       <c r="C25" s="6" t="s">
         <v>41</v>
@@ -1151,7 +1168,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="3"/>
       <c r="C26" s="6" t="s">
         <v>42</v>
@@ -1162,7 +1179,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="3"/>
       <c r="C27" s="6" t="s">
         <v>43</v>
@@ -1173,7 +1190,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="3"/>
       <c r="C28" s="6" t="s">
         <v>44</v>
@@ -1184,7 +1201,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="3"/>
       <c r="C29" s="6" t="s">
         <v>45</v>
@@ -1195,7 +1212,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="9" t="s">
         <v>35</v>
       </c>
@@ -1206,7 +1223,7 @@
       <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="3"/>
       <c r="C31" s="6" t="s">
         <v>41</v>
@@ -1217,7 +1234,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="3"/>
       <c r="C32" s="6" t="s">
         <v>42</v>
@@ -1228,7 +1245,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="3"/>
       <c r="C33" s="6" t="s">
         <v>43</v>
@@ -1239,7 +1256,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
+      <c r="A34" s="27"/>
       <c r="B34" s="3"/>
       <c r="C34" s="6" t="s">
         <v>44</v>
@@ -1250,7 +1267,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="A35" s="27"/>
       <c r="B35" s="3"/>
       <c r="C35" s="6" t="s">
         <v>45</v>
@@ -1261,7 +1278,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
+      <c r="A36" s="27"/>
       <c r="B36" s="9" t="s">
         <v>36</v>
       </c>
@@ -1272,7 +1289,7 @@
       <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="3"/>
       <c r="C37" s="6" t="s">
         <v>41</v>
@@ -1283,7 +1300,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
+      <c r="A38" s="27"/>
       <c r="B38" s="3"/>
       <c r="C38" s="6" t="s">
         <v>42</v>
@@ -1294,7 +1311,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
+      <c r="A39" s="27"/>
       <c r="B39" s="3"/>
       <c r="C39" s="6" t="s">
         <v>43</v>
@@ -1305,7 +1322,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
+      <c r="A40" s="27"/>
       <c r="B40" s="3"/>
       <c r="C40" s="6" t="s">
         <v>44</v>
@@ -1316,7 +1333,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
+      <c r="A41" s="27"/>
       <c r="B41" s="3"/>
       <c r="C41" s="6" t="s">
         <v>45</v>
@@ -1327,7 +1344,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+      <c r="A42" s="27"/>
       <c r="B42" s="9" t="s">
         <v>37</v>
       </c>
@@ -1338,7 +1355,7 @@
       <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
+      <c r="A43" s="27"/>
       <c r="B43" s="3"/>
       <c r="C43" s="6" t="s">
         <v>41</v>
@@ -1349,7 +1366,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+      <c r="A44" s="27"/>
       <c r="B44" s="3"/>
       <c r="C44" s="6" t="s">
         <v>42</v>
@@ -1360,7 +1377,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="26"/>
+      <c r="A45" s="27"/>
       <c r="B45" s="3"/>
       <c r="C45" s="6" t="s">
         <v>43</v>
@@ -1371,7 +1388,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
+      <c r="A46" s="27"/>
       <c r="B46" s="3"/>
       <c r="C46" s="6" t="s">
         <v>44</v>
@@ -1382,7 +1399,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
+      <c r="A47" s="27"/>
       <c r="B47" s="3"/>
       <c r="C47" s="6" t="s">
         <v>45</v>
@@ -1393,7 +1410,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A48" s="26"/>
+      <c r="A48" s="27"/>
       <c r="B48" s="9" t="s">
         <v>38</v>
       </c>
@@ -1404,7 +1421,7 @@
       <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="26"/>
+      <c r="A49" s="27"/>
       <c r="B49" s="3"/>
       <c r="C49" s="6" t="s">
         <v>41</v>
@@ -1415,7 +1432,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="26"/>
+      <c r="A50" s="27"/>
       <c r="B50" s="3"/>
       <c r="C50" s="6" t="s">
         <v>42</v>
@@ -1426,7 +1443,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="26"/>
+      <c r="A51" s="27"/>
       <c r="B51" s="3"/>
       <c r="C51" s="6" t="s">
         <v>43</v>
@@ -1437,7 +1454,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
+      <c r="A52" s="27"/>
       <c r="B52" s="3"/>
       <c r="C52" s="6" t="s">
         <v>44</v>
@@ -1448,7 +1465,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="26"/>
+      <c r="A53" s="27"/>
       <c r="B53" s="3"/>
       <c r="C53" s="6" t="s">
         <v>45</v>
@@ -1459,7 +1476,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A54" s="26"/>
+      <c r="A54" s="27"/>
       <c r="B54" s="9" t="s">
         <v>39</v>
       </c>
@@ -1470,7 +1487,7 @@
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
+      <c r="A55" s="27"/>
       <c r="B55" s="3"/>
       <c r="C55" s="6" t="s">
         <v>41</v>
@@ -1481,7 +1498,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="26"/>
+      <c r="A56" s="27"/>
       <c r="B56" s="3"/>
       <c r="C56" s="6" t="s">
         <v>42</v>
@@ -1492,7 +1509,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
+      <c r="A57" s="27"/>
       <c r="B57" s="3"/>
       <c r="C57" s="6" t="s">
         <v>43</v>
@@ -1503,7 +1520,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="26"/>
+      <c r="A58" s="27"/>
       <c r="B58" s="3"/>
       <c r="C58" s="6" t="s">
         <v>44</v>
@@ -1514,7 +1531,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="26"/>
+      <c r="A59" s="27"/>
       <c r="B59" s="3"/>
       <c r="C59" s="6" t="s">
         <v>45</v>
@@ -1525,7 +1542,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="26"/>
+      <c r="A60" s="27"/>
       <c r="B60" s="9" t="s">
         <v>40</v>
       </c>
@@ -1536,7 +1553,7 @@
       <c r="E60" s="7"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="26"/>
+      <c r="A61" s="27"/>
       <c r="B61" s="3"/>
       <c r="C61" s="6" t="s">
         <v>41</v>
@@ -1547,7 +1564,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="26"/>
+      <c r="A62" s="27"/>
       <c r="B62" s="3"/>
       <c r="C62" s="6" t="s">
         <v>42</v>
@@ -1558,7 +1575,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="26"/>
+      <c r="A63" s="27"/>
       <c r="B63" s="3"/>
       <c r="C63" s="6" t="s">
         <v>43</v>
@@ -1569,7 +1586,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="26"/>
+      <c r="A64" s="27"/>
       <c r="B64" s="3"/>
       <c r="C64" s="6" t="s">
         <v>44</v>
@@ -1580,7 +1597,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="26"/>
+      <c r="A65" s="27"/>
       <c r="B65" s="3"/>
       <c r="C65" s="6" t="s">
         <v>45</v>
@@ -1591,7 +1608,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="26"/>
+      <c r="A66" s="27"/>
       <c r="B66" s="6" t="s">
         <v>54</v>
       </c>
@@ -1602,7 +1619,7 @@
       <c r="E66" s="7"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="26"/>
+      <c r="A67" s="27"/>
       <c r="B67" s="3"/>
       <c r="C67" s="6" t="s">
         <v>56</v>
@@ -1613,7 +1630,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="27"/>
+      <c r="A68" s="28"/>
       <c r="B68" s="10"/>
       <c r="C68" s="11" t="s">
         <v>55</v>
@@ -1624,7 +1641,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A69" s="25" t="s">
+      <c r="A69" s="26" t="s">
         <v>53</v>
       </c>
       <c r="B69" s="4" t="s">
@@ -1637,7 +1654,7 @@
       <c r="E69" s="5"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="26"/>
+      <c r="A70" s="27"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6" t="s">
         <v>58</v>
@@ -1648,7 +1665,7 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="26"/>
+      <c r="A71" s="27"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6" t="s">
         <v>59</v>
@@ -1659,7 +1676,7 @@
       </c>
     </row>
     <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="26"/>
+      <c r="A72" s="27"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6" t="s">
         <v>60</v>
@@ -1670,7 +1687,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="26"/>
+      <c r="A73" s="27"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6" t="s">
         <v>61</v>
@@ -1681,7 +1698,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="26"/>
+      <c r="A74" s="27"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6" t="s">
         <v>62</v>
@@ -1692,7 +1709,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A75" s="26"/>
+      <c r="A75" s="27"/>
       <c r="B75" s="6" t="s">
         <v>64</v>
       </c>
@@ -1703,7 +1720,7 @@
       <c r="E75" s="7"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="26"/>
+      <c r="A76" s="27"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6" t="s">
         <v>58</v>
@@ -1714,7 +1731,7 @@
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="26"/>
+      <c r="A77" s="27"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6" t="s">
         <v>59</v>
@@ -1725,7 +1742,7 @@
       </c>
     </row>
     <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="26"/>
+      <c r="A78" s="27"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6" t="s">
         <v>60</v>
@@ -1736,7 +1753,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="26"/>
+      <c r="A79" s="27"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6" t="s">
         <v>61</v>
@@ -1747,7 +1764,7 @@
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="26"/>
+      <c r="A80" s="27"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6" t="s">
         <v>62</v>
@@ -1758,7 +1775,7 @@
       </c>
     </row>
     <row r="81" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A81" s="26"/>
+      <c r="A81" s="27"/>
       <c r="B81" s="6" t="s">
         <v>65</v>
       </c>
@@ -1769,7 +1786,7 @@
       <c r="E81" s="7"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="26"/>
+      <c r="A82" s="27"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6" t="s">
         <v>58</v>
@@ -1780,7 +1797,7 @@
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="26"/>
+      <c r="A83" s="27"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6" t="s">
         <v>59</v>
@@ -1791,7 +1808,7 @@
       </c>
     </row>
     <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="26"/>
+      <c r="A84" s="27"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6" t="s">
         <v>60</v>
@@ -1802,7 +1819,7 @@
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="26"/>
+      <c r="A85" s="27"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6" t="s">
         <v>61</v>
@@ -1813,7 +1830,7 @@
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="26"/>
+      <c r="A86" s="27"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6" t="s">
         <v>62</v>
@@ -1824,7 +1841,7 @@
       </c>
     </row>
     <row r="87" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A87" s="26"/>
+      <c r="A87" s="27"/>
       <c r="B87" s="6" t="s">
         <v>69</v>
       </c>
@@ -1835,7 +1852,7 @@
       <c r="E87" s="7"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="26"/>
+      <c r="A88" s="27"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6" t="s">
         <v>58</v>
@@ -1846,7 +1863,7 @@
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="26"/>
+      <c r="A89" s="27"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6" t="s">
         <v>59</v>
@@ -1857,7 +1874,7 @@
       </c>
     </row>
     <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="26"/>
+      <c r="A90" s="27"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6" t="s">
         <v>60</v>
@@ -1868,7 +1885,7 @@
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="26"/>
+      <c r="A91" s="27"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6" t="s">
         <v>61</v>
@@ -1879,7 +1896,7 @@
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="26"/>
+      <c r="A92" s="27"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6" t="s">
         <v>62</v>
@@ -1890,7 +1907,7 @@
       </c>
     </row>
     <row r="93" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A93" s="26"/>
+      <c r="A93" s="27"/>
       <c r="B93" s="6" t="s">
         <v>71</v>
       </c>
@@ -1901,7 +1918,7 @@
       <c r="E93" s="7"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="26"/>
+      <c r="A94" s="27"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6" t="s">
         <v>58</v>
@@ -1912,7 +1929,7 @@
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="26"/>
+      <c r="A95" s="27"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6" t="s">
         <v>59</v>
@@ -1923,7 +1940,7 @@
       </c>
     </row>
     <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A96" s="26"/>
+      <c r="A96" s="27"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6" t="s">
         <v>60</v>
@@ -1934,7 +1951,7 @@
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="26"/>
+      <c r="A97" s="27"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6" t="s">
         <v>61</v>
@@ -1945,7 +1962,7 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="26"/>
+      <c r="A98" s="27"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6" t="s">
         <v>62</v>
@@ -1956,7 +1973,7 @@
       </c>
     </row>
     <row r="99" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A99" s="26"/>
+      <c r="A99" s="27"/>
       <c r="B99" s="6" t="s">
         <v>73</v>
       </c>
@@ -1967,7 +1984,7 @@
       <c r="E99" s="7"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="26"/>
+      <c r="A100" s="27"/>
       <c r="B100" s="6"/>
       <c r="C100" s="6" t="s">
         <v>58</v>
@@ -1978,7 +1995,7 @@
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="26"/>
+      <c r="A101" s="27"/>
       <c r="B101" s="6"/>
       <c r="C101" s="6" t="s">
         <v>59</v>
@@ -1989,7 +2006,7 @@
       </c>
     </row>
     <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A102" s="26"/>
+      <c r="A102" s="27"/>
       <c r="B102" s="6"/>
       <c r="C102" s="6" t="s">
         <v>60</v>
@@ -2000,7 +2017,7 @@
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="26"/>
+      <c r="A103" s="27"/>
       <c r="B103" s="6"/>
       <c r="C103" s="6" t="s">
         <v>61</v>
@@ -2011,7 +2028,7 @@
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="26"/>
+      <c r="A104" s="27"/>
       <c r="B104" s="6"/>
       <c r="C104" s="6" t="s">
         <v>62</v>
@@ -2022,7 +2039,7 @@
       </c>
     </row>
     <row r="105" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A105" s="26"/>
+      <c r="A105" s="27"/>
       <c r="B105" s="6" t="s">
         <v>75</v>
       </c>
@@ -2033,7 +2050,7 @@
       <c r="E105" s="7"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="26"/>
+      <c r="A106" s="27"/>
       <c r="B106" s="6"/>
       <c r="C106" s="6" t="s">
         <v>58</v>
@@ -2044,7 +2061,7 @@
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="26"/>
+      <c r="A107" s="27"/>
       <c r="B107" s="6"/>
       <c r="C107" s="6" t="s">
         <v>59</v>
@@ -2055,7 +2072,7 @@
       </c>
     </row>
     <row r="108" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="26"/>
+      <c r="A108" s="27"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6" t="s">
         <v>60</v>
@@ -2066,7 +2083,7 @@
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="26"/>
+      <c r="A109" s="27"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6" t="s">
         <v>61</v>
@@ -2077,7 +2094,7 @@
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="26"/>
+      <c r="A110" s="27"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6" t="s">
         <v>62</v>
@@ -2088,7 +2105,7 @@
       </c>
     </row>
     <row r="111" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A111" s="26"/>
+      <c r="A111" s="27"/>
       <c r="B111" s="6" t="s">
         <v>77</v>
       </c>
@@ -2099,7 +2116,7 @@
       <c r="E111" s="7"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="26"/>
+      <c r="A112" s="27"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6" t="s">
         <v>58</v>
@@ -2110,7 +2127,7 @@
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="26"/>
+      <c r="A113" s="27"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6" t="s">
         <v>59</v>
@@ -2121,7 +2138,7 @@
       </c>
     </row>
     <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="26"/>
+      <c r="A114" s="27"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6" t="s">
         <v>60</v>
@@ -2132,7 +2149,7 @@
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="26"/>
+      <c r="A115" s="27"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6" t="s">
         <v>61</v>
@@ -2143,7 +2160,7 @@
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="26"/>
+      <c r="A116" s="27"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6" t="s">
         <v>62</v>
@@ -2154,7 +2171,7 @@
       </c>
     </row>
     <row r="117" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A117" s="26"/>
+      <c r="A117" s="27"/>
       <c r="B117" s="6" t="s">
         <v>79</v>
       </c>
@@ -2165,7 +2182,7 @@
       <c r="E117" s="7"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="26"/>
+      <c r="A118" s="27"/>
       <c r="B118" s="6"/>
       <c r="C118" s="6" t="s">
         <v>58</v>
@@ -2176,7 +2193,7 @@
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="26"/>
+      <c r="A119" s="27"/>
       <c r="B119" s="6"/>
       <c r="C119" s="6" t="s">
         <v>59</v>
@@ -2187,7 +2204,7 @@
       </c>
     </row>
     <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="26"/>
+      <c r="A120" s="27"/>
       <c r="B120" s="6"/>
       <c r="C120" s="6" t="s">
         <v>60</v>
@@ -2198,7 +2215,7 @@
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="26"/>
+      <c r="A121" s="27"/>
       <c r="B121" s="6"/>
       <c r="C121" s="6" t="s">
         <v>61</v>
@@ -2209,7 +2226,7 @@
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="26"/>
+      <c r="A122" s="27"/>
       <c r="B122" s="6"/>
       <c r="C122" s="6" t="s">
         <v>62</v>
@@ -2220,7 +2237,7 @@
       </c>
     </row>
     <row r="123" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A123" s="26"/>
+      <c r="A123" s="27"/>
       <c r="B123" s="6" t="s">
         <v>81</v>
       </c>
@@ -2231,7 +2248,7 @@
       <c r="E123" s="7"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="26"/>
+      <c r="A124" s="27"/>
       <c r="B124" s="6"/>
       <c r="C124" s="6" t="s">
         <v>58</v>
@@ -2242,7 +2259,7 @@
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="26"/>
+      <c r="A125" s="27"/>
       <c r="B125" s="6"/>
       <c r="C125" s="6" t="s">
         <v>59</v>
@@ -2253,7 +2270,7 @@
       </c>
     </row>
     <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A126" s="26"/>
+      <c r="A126" s="27"/>
       <c r="B126" s="6"/>
       <c r="C126" s="6" t="s">
         <v>60</v>
@@ -2264,7 +2281,7 @@
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="26"/>
+      <c r="A127" s="27"/>
       <c r="B127" s="6"/>
       <c r="C127" s="6" t="s">
         <v>61</v>
@@ -2275,7 +2292,7 @@
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" s="26"/>
+      <c r="A128" s="27"/>
       <c r="B128" s="6"/>
       <c r="C128" s="6" t="s">
         <v>62</v>
@@ -2286,7 +2303,7 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="27"/>
+      <c r="A129" s="28"/>
       <c r="B129" s="11"/>
       <c r="C129" s="11"/>
       <c r="D129" s="11"/>
@@ -2302,7 +2319,7 @@
       </c>
     </row>
     <row r="131" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A131" s="26" t="s">
+      <c r="A131" s="27" t="s">
         <v>83</v>
       </c>
       <c r="B131" s="6" t="s">
@@ -2315,7 +2332,7 @@
       <c r="E131" s="7"/>
     </row>
     <row r="132" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A132" s="26"/>
+      <c r="A132" s="27"/>
       <c r="B132" s="6"/>
       <c r="C132" s="6" t="s">
         <v>85</v>
@@ -2326,7 +2343,7 @@
       </c>
     </row>
     <row r="133" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A133" s="26"/>
+      <c r="A133" s="27"/>
       <c r="B133" s="6"/>
       <c r="C133" s="6" t="s">
         <v>86</v>
@@ -2337,7 +2354,7 @@
       </c>
     </row>
     <row r="134" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A134" s="26"/>
+      <c r="A134" s="27"/>
       <c r="B134" s="6" t="s">
         <v>84</v>
       </c>
@@ -2348,7 +2365,7 @@
       <c r="E134" s="7"/>
     </row>
     <row r="135" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A135" s="26"/>
+      <c r="A135" s="27"/>
       <c r="B135" s="6"/>
       <c r="C135" s="6" t="s">
         <v>87</v>
@@ -2359,7 +2376,7 @@
       </c>
     </row>
     <row r="136" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A136" s="26"/>
+      <c r="A136" s="27"/>
       <c r="B136" s="6"/>
       <c r="C136" s="6" t="s">
         <v>88</v>
@@ -2370,7 +2387,7 @@
       </c>
     </row>
     <row r="137" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A137" s="26"/>
+      <c r="A137" s="27"/>
       <c r="B137" s="6" t="s">
         <v>84</v>
       </c>
@@ -2381,7 +2398,7 @@
       <c r="E137" s="7"/>
     </row>
     <row r="138" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A138" s="26"/>
+      <c r="A138" s="27"/>
       <c r="B138" s="6"/>
       <c r="C138" s="6" t="s">
         <v>89</v>
@@ -2392,7 +2409,7 @@
       </c>
     </row>
     <row r="139" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A139" s="26"/>
+      <c r="A139" s="27"/>
       <c r="B139" s="6"/>
       <c r="C139" s="6" t="s">
         <v>90</v>
@@ -2403,7 +2420,7 @@
       </c>
     </row>
     <row r="140" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A140" s="26"/>
+      <c r="A140" s="27"/>
       <c r="B140" s="6" t="s">
         <v>84</v>
       </c>
@@ -2414,7 +2431,7 @@
       <c r="E140" s="7"/>
     </row>
     <row r="141" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A141" s="26"/>
+      <c r="A141" s="27"/>
       <c r="B141" s="6"/>
       <c r="C141" s="6" t="s">
         <v>91</v>
@@ -2425,7 +2442,7 @@
       </c>
     </row>
     <row r="142" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A142" s="26"/>
+      <c r="A142" s="27"/>
       <c r="B142" s="6"/>
       <c r="C142" s="6" t="s">
         <v>92</v>
@@ -2436,7 +2453,7 @@
       </c>
     </row>
     <row r="143" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A143" s="26"/>
+      <c r="A143" s="27"/>
       <c r="B143" s="6" t="s">
         <v>84</v>
       </c>
@@ -2447,7 +2464,7 @@
       <c r="E143" s="7"/>
     </row>
     <row r="144" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A144" s="26"/>
+      <c r="A144" s="27"/>
       <c r="B144" s="6"/>
       <c r="C144" s="6" t="s">
         <v>93</v>
@@ -2458,7 +2475,7 @@
       </c>
     </row>
     <row r="145" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A145" s="26"/>
+      <c r="A145" s="27"/>
       <c r="B145" s="6"/>
       <c r="C145" s="6" t="s">
         <v>94</v>
@@ -2469,7 +2486,7 @@
       </c>
     </row>
     <row r="146" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A146" s="26"/>
+      <c r="A146" s="27"/>
       <c r="B146" s="6" t="s">
         <v>84</v>
       </c>
@@ -2480,7 +2497,7 @@
       <c r="E146" s="7"/>
     </row>
     <row r="147" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A147" s="26"/>
+      <c r="A147" s="27"/>
       <c r="B147" s="6"/>
       <c r="C147" s="6" t="s">
         <v>95</v>
@@ -2491,7 +2508,7 @@
       </c>
     </row>
     <row r="148" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A148" s="26"/>
+      <c r="A148" s="27"/>
       <c r="B148" s="6"/>
       <c r="C148" s="6" t="s">
         <v>96</v>
@@ -2502,7 +2519,7 @@
       </c>
     </row>
     <row r="149" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A149" s="26"/>
+      <c r="A149" s="27"/>
       <c r="B149" s="6" t="s">
         <v>84</v>
       </c>
@@ -2513,7 +2530,7 @@
       <c r="E149" s="7"/>
     </row>
     <row r="150" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A150" s="26"/>
+      <c r="A150" s="27"/>
       <c r="B150" s="6"/>
       <c r="C150" s="6" t="s">
         <v>97</v>
@@ -2524,7 +2541,7 @@
       </c>
     </row>
     <row r="151" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A151" s="26"/>
+      <c r="A151" s="27"/>
       <c r="B151" s="6"/>
       <c r="C151" s="6" t="s">
         <v>98</v>
@@ -2535,7 +2552,7 @@
       </c>
     </row>
     <row r="152" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A152" s="26"/>
+      <c r="A152" s="27"/>
       <c r="B152" s="6" t="s">
         <v>84</v>
       </c>
@@ -2546,7 +2563,7 @@
       <c r="E152" s="7"/>
     </row>
     <row r="153" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A153" s="26"/>
+      <c r="A153" s="27"/>
       <c r="B153" s="6"/>
       <c r="C153" s="6" t="s">
         <v>99</v>
@@ -2557,7 +2574,7 @@
       </c>
     </row>
     <row r="154" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A154" s="26"/>
+      <c r="A154" s="27"/>
       <c r="B154" s="6"/>
       <c r="C154" s="6" t="s">
         <v>100</v>
@@ -2568,7 +2585,7 @@
       </c>
     </row>
     <row r="155" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A155" s="26"/>
+      <c r="A155" s="27"/>
       <c r="B155" s="6" t="s">
         <v>84</v>
       </c>
@@ -2579,7 +2596,7 @@
       <c r="E155" s="7"/>
     </row>
     <row r="156" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A156" s="26"/>
+      <c r="A156" s="27"/>
       <c r="B156" s="6"/>
       <c r="C156" s="6" t="s">
         <v>101</v>
@@ -2590,7 +2607,7 @@
       </c>
     </row>
     <row r="157" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A157" s="26"/>
+      <c r="A157" s="27"/>
       <c r="B157" s="6"/>
       <c r="C157" s="6" t="s">
         <v>102</v>
@@ -2601,7 +2618,7 @@
       </c>
     </row>
     <row r="158" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A158" s="26"/>
+      <c r="A158" s="27"/>
       <c r="B158" s="6" t="s">
         <v>84</v>
       </c>
@@ -2612,7 +2629,7 @@
       <c r="E158" s="7"/>
     </row>
     <row r="159" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A159" s="26"/>
+      <c r="A159" s="27"/>
       <c r="B159" s="6"/>
       <c r="C159" s="6" t="s">
         <v>103</v>
@@ -2623,7 +2640,7 @@
       </c>
     </row>
     <row r="160" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="27"/>
+      <c r="A160" s="28"/>
       <c r="B160" s="11"/>
       <c r="C160" s="11" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
nettoyage data non utilisées
</commit_message>
<xml_diff>
--- a/xp/log_questionnaire_XP_WEEK2_EXPLAINED.xlsx
+++ b/xp/log_questionnaire_XP_WEEK2_EXPLAINED.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="0" windowWidth="27780" windowHeight="12285"/>
+    <workbookView xWindow="4800" yWindow="0" windowWidth="27780" windowHeight="12285"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="121">
   <si>
     <t>Questionnaire rewrite</t>
   </si>
@@ -378,6 +378,15 @@
   </si>
   <si>
     <t>GLOBAL : transformer toutes les , en _</t>
+  </si>
+  <si>
+    <t>profil joueur jeux favoris</t>
+  </si>
+  <si>
+    <t>Citez trois de vos jeux favoris en précisant leur support (jeu vidéo, jeu de plateau/de société, etc.) :</t>
+  </si>
+  <si>
+    <t>jeuxFav</t>
   </si>
 </sst>
 </file>
@@ -513,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -589,6 +598,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -879,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E160"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,7 +934,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="27" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -935,7 +947,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
@@ -946,7 +958,7 @@
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
@@ -957,7 +969,7 @@
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
@@ -968,7 +980,7 @@
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="19" t="s">
         <v>10</v>
       </c>
@@ -979,7 +991,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="20"/>
       <c r="C9" s="6" t="s">
         <v>31</v>
@@ -990,7 +1002,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="21"/>
       <c r="C10" s="11" t="s">
         <v>32</v>
@@ -1001,7 +1013,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="9" t="s">
         <v>11</v>
       </c>
@@ -1012,7 +1024,7 @@
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="9"/>
       <c r="C12" s="6" t="s">
         <v>29</v>
@@ -1023,7 +1035,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="27"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="9"/>
       <c r="C13" s="6" t="s">
         <v>30</v>
@@ -1034,7 +1046,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="22" t="s">
         <v>12</v>
       </c>
@@ -1045,7 +1057,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="23"/>
       <c r="C15" s="6" t="s">
         <v>20</v>
@@ -1056,7 +1068,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="23"/>
       <c r="C16" s="6" t="s">
         <v>21</v>
@@ -1067,7 +1079,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="23"/>
       <c r="C17" s="6" t="s">
         <v>22</v>
@@ -1078,7 +1090,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="23"/>
       <c r="C18" s="6" t="s">
         <v>23</v>
@@ -1089,7 +1101,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="23"/>
       <c r="C19" s="6" t="s">
         <v>24</v>
@@ -1100,7 +1112,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="23"/>
       <c r="C20" s="6" t="s">
         <v>25</v>
@@ -1111,7 +1123,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="23"/>
       <c r="C21" s="6" t="s">
         <v>26</v>
@@ -1122,7 +1134,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="23"/>
       <c r="C22" s="6" t="s">
         <v>27</v>
@@ -1133,7 +1145,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="28"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="24"/>
       <c r="C23" s="17" t="s">
         <v>28</v>
@@ -1144,7 +1156,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1157,7 +1169,7 @@
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="3"/>
       <c r="C25" s="6" t="s">
         <v>41</v>
@@ -1168,7 +1180,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="3"/>
       <c r="C26" s="6" t="s">
         <v>42</v>
@@ -1179,7 +1191,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="3"/>
       <c r="C27" s="6" t="s">
         <v>43</v>
@@ -1190,7 +1202,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="3"/>
       <c r="C28" s="6" t="s">
         <v>44</v>
@@ -1201,7 +1213,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="3"/>
       <c r="C29" s="6" t="s">
         <v>45</v>
@@ -1212,7 +1224,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="9" t="s">
         <v>35</v>
       </c>
@@ -1223,7 +1235,7 @@
       <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="3"/>
       <c r="C31" s="6" t="s">
         <v>41</v>
@@ -1234,7 +1246,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="3"/>
       <c r="C32" s="6" t="s">
         <v>42</v>
@@ -1245,7 +1257,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="3"/>
       <c r="C33" s="6" t="s">
         <v>43</v>
@@ -1256,7 +1268,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
+      <c r="A34" s="28"/>
       <c r="B34" s="3"/>
       <c r="C34" s="6" t="s">
         <v>44</v>
@@ -1267,7 +1279,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
+      <c r="A35" s="28"/>
       <c r="B35" s="3"/>
       <c r="C35" s="6" t="s">
         <v>45</v>
@@ -1278,7 +1290,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
+      <c r="A36" s="28"/>
       <c r="B36" s="9" t="s">
         <v>36</v>
       </c>
@@ -1289,7 +1301,7 @@
       <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="27"/>
+      <c r="A37" s="28"/>
       <c r="B37" s="3"/>
       <c r="C37" s="6" t="s">
         <v>41</v>
@@ -1300,7 +1312,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="27"/>
+      <c r="A38" s="28"/>
       <c r="B38" s="3"/>
       <c r="C38" s="6" t="s">
         <v>42</v>
@@ -1311,7 +1323,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
+      <c r="A39" s="28"/>
       <c r="B39" s="3"/>
       <c r="C39" s="6" t="s">
         <v>43</v>
@@ -1322,7 +1334,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
+      <c r="A40" s="28"/>
       <c r="B40" s="3"/>
       <c r="C40" s="6" t="s">
         <v>44</v>
@@ -1333,7 +1345,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="27"/>
+      <c r="A41" s="28"/>
       <c r="B41" s="3"/>
       <c r="C41" s="6" t="s">
         <v>45</v>
@@ -1344,7 +1356,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="27"/>
+      <c r="A42" s="28"/>
       <c r="B42" s="9" t="s">
         <v>37</v>
       </c>
@@ -1355,7 +1367,7 @@
       <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="27"/>
+      <c r="A43" s="28"/>
       <c r="B43" s="3"/>
       <c r="C43" s="6" t="s">
         <v>41</v>
@@ -1366,7 +1378,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="27"/>
+      <c r="A44" s="28"/>
       <c r="B44" s="3"/>
       <c r="C44" s="6" t="s">
         <v>42</v>
@@ -1377,7 +1389,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="27"/>
+      <c r="A45" s="28"/>
       <c r="B45" s="3"/>
       <c r="C45" s="6" t="s">
         <v>43</v>
@@ -1388,7 +1400,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="27"/>
+      <c r="A46" s="28"/>
       <c r="B46" s="3"/>
       <c r="C46" s="6" t="s">
         <v>44</v>
@@ -1399,7 +1411,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="27"/>
+      <c r="A47" s="28"/>
       <c r="B47" s="3"/>
       <c r="C47" s="6" t="s">
         <v>45</v>
@@ -1410,7 +1422,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A48" s="27"/>
+      <c r="A48" s="28"/>
       <c r="B48" s="9" t="s">
         <v>38</v>
       </c>
@@ -1421,7 +1433,7 @@
       <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="27"/>
+      <c r="A49" s="28"/>
       <c r="B49" s="3"/>
       <c r="C49" s="6" t="s">
         <v>41</v>
@@ -1432,7 +1444,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="27"/>
+      <c r="A50" s="28"/>
       <c r="B50" s="3"/>
       <c r="C50" s="6" t="s">
         <v>42</v>
@@ -1443,7 +1455,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="27"/>
+      <c r="A51" s="28"/>
       <c r="B51" s="3"/>
       <c r="C51" s="6" t="s">
         <v>43</v>
@@ -1454,7 +1466,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="27"/>
+      <c r="A52" s="28"/>
       <c r="B52" s="3"/>
       <c r="C52" s="6" t="s">
         <v>44</v>
@@ -1465,7 +1477,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="27"/>
+      <c r="A53" s="28"/>
       <c r="B53" s="3"/>
       <c r="C53" s="6" t="s">
         <v>45</v>
@@ -1476,7 +1488,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A54" s="27"/>
+      <c r="A54" s="28"/>
       <c r="B54" s="9" t="s">
         <v>39</v>
       </c>
@@ -1487,7 +1499,7 @@
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="27"/>
+      <c r="A55" s="28"/>
       <c r="B55" s="3"/>
       <c r="C55" s="6" t="s">
         <v>41</v>
@@ -1498,7 +1510,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="27"/>
+      <c r="A56" s="28"/>
       <c r="B56" s="3"/>
       <c r="C56" s="6" t="s">
         <v>42</v>
@@ -1509,7 +1521,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="27"/>
+      <c r="A57" s="28"/>
       <c r="B57" s="3"/>
       <c r="C57" s="6" t="s">
         <v>43</v>
@@ -1520,7 +1532,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="27"/>
+      <c r="A58" s="28"/>
       <c r="B58" s="3"/>
       <c r="C58" s="6" t="s">
         <v>44</v>
@@ -1531,7 +1543,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="27"/>
+      <c r="A59" s="28"/>
       <c r="B59" s="3"/>
       <c r="C59" s="6" t="s">
         <v>45</v>
@@ -1542,7 +1554,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="27"/>
+      <c r="A60" s="28"/>
       <c r="B60" s="9" t="s">
         <v>40</v>
       </c>
@@ -1553,7 +1565,7 @@
       <c r="E60" s="7"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="27"/>
+      <c r="A61" s="28"/>
       <c r="B61" s="3"/>
       <c r="C61" s="6" t="s">
         <v>41</v>
@@ -1564,7 +1576,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="27"/>
+      <c r="A62" s="28"/>
       <c r="B62" s="3"/>
       <c r="C62" s="6" t="s">
         <v>42</v>
@@ -1575,7 +1587,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="27"/>
+      <c r="A63" s="28"/>
       <c r="B63" s="3"/>
       <c r="C63" s="6" t="s">
         <v>43</v>
@@ -1586,7 +1598,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="27"/>
+      <c r="A64" s="28"/>
       <c r="B64" s="3"/>
       <c r="C64" s="6" t="s">
         <v>44</v>
@@ -1597,7 +1609,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="27"/>
+      <c r="A65" s="28"/>
       <c r="B65" s="3"/>
       <c r="C65" s="6" t="s">
         <v>45</v>
@@ -1608,7 +1620,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="27"/>
+      <c r="A66" s="28"/>
       <c r="B66" s="6" t="s">
         <v>54</v>
       </c>
@@ -1619,7 +1631,7 @@
       <c r="E66" s="7"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="27"/>
+      <c r="A67" s="28"/>
       <c r="B67" s="3"/>
       <c r="C67" s="6" t="s">
         <v>56</v>
@@ -1630,7 +1642,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="28"/>
+      <c r="A68" s="29"/>
       <c r="B68" s="10"/>
       <c r="C68" s="11" t="s">
         <v>55</v>
@@ -1640,1020 +1652,1033 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E69" s="7"/>
+    </row>
+    <row r="70" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A70" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4" t="s">
+      <c r="C70" s="4"/>
+      <c r="D70" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E69" s="5"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="27"/>
-      <c r="B70" s="6"/>
-      <c r="C70" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D70" s="6"/>
-      <c r="E70" s="7">
-        <v>1</v>
-      </c>
+      <c r="E70" s="5"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="27"/>
+      <c r="A71" s="28"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="28"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="27"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="28"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="27"/>
+      <c r="A74" s="28"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="28"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D75" s="6"/>
+      <c r="E75" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A75" s="27"/>
-      <c r="B75" s="6" t="s">
+    <row r="76" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A76" s="28"/>
+      <c r="B76" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C75" s="6"/>
-      <c r="D75" s="6" t="s">
+      <c r="C76" s="6"/>
+      <c r="D76" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E75" s="7"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="27"/>
-      <c r="B76" s="6"/>
-      <c r="C76" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D76" s="6"/>
-      <c r="E76" s="7">
-        <v>1</v>
-      </c>
+      <c r="E76" s="7"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="27"/>
+      <c r="A77" s="28"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="28"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="27"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="28"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="27"/>
+      <c r="A80" s="28"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="28"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D81" s="6"/>
+      <c r="E81" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A81" s="27"/>
-      <c r="B81" s="6" t="s">
+    <row r="82" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A82" s="28"/>
+      <c r="B82" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C81" s="6"/>
-      <c r="D81" s="6" t="s">
+      <c r="C82" s="6"/>
+      <c r="D82" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E81" s="7"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="27"/>
-      <c r="B82" s="6"/>
-      <c r="C82" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D82" s="6"/>
-      <c r="E82" s="7">
-        <v>1</v>
-      </c>
+      <c r="E82" s="7"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="27"/>
+      <c r="A83" s="28"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D83" s="6"/>
       <c r="E83" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="28"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D84" s="6"/>
       <c r="E84" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="27"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="28"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D85" s="6"/>
       <c r="E85" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="27"/>
+      <c r="A86" s="28"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D86" s="6"/>
       <c r="E86" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="28"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D87" s="6"/>
+      <c r="E87" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A87" s="27"/>
-      <c r="B87" s="6" t="s">
+    <row r="88" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A88" s="28"/>
+      <c r="B88" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C87" s="6"/>
-      <c r="D87" s="6" t="s">
+      <c r="C88" s="6"/>
+      <c r="D88" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E87" s="7"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="27"/>
-      <c r="B88" s="6"/>
-      <c r="C88" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D88" s="6"/>
-      <c r="E88" s="7">
-        <v>1</v>
-      </c>
+      <c r="E88" s="7"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="27"/>
+      <c r="A89" s="28"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D89" s="6"/>
       <c r="E89" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="28"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D90" s="6"/>
       <c r="E90" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="27"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="28"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D91" s="6"/>
       <c r="E91" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="27"/>
+      <c r="A92" s="28"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D92" s="6"/>
       <c r="E92" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="28"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D93" s="6"/>
+      <c r="E93" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A93" s="27"/>
-      <c r="B93" s="6" t="s">
+    <row r="94" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A94" s="28"/>
+      <c r="B94" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C93" s="6"/>
-      <c r="D93" s="6" t="s">
+      <c r="C94" s="6"/>
+      <c r="D94" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E93" s="7"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="27"/>
-      <c r="B94" s="6"/>
-      <c r="C94" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D94" s="6"/>
-      <c r="E94" s="7">
-        <v>1</v>
-      </c>
+      <c r="E94" s="7"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="27"/>
+      <c r="A95" s="28"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D95" s="6"/>
       <c r="E95" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A96" s="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="28"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D96" s="6"/>
       <c r="E96" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="27"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="28"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D97" s="6"/>
       <c r="E97" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="27"/>
+      <c r="A98" s="28"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D98" s="6"/>
       <c r="E98" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="28"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D99" s="6"/>
+      <c r="E99" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A99" s="27"/>
-      <c r="B99" s="6" t="s">
+    <row r="100" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A100" s="28"/>
+      <c r="B100" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C99" s="6"/>
-      <c r="D99" s="6" t="s">
+      <c r="C100" s="6"/>
+      <c r="D100" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E99" s="7"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="27"/>
-      <c r="B100" s="6"/>
-      <c r="C100" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D100" s="6"/>
-      <c r="E100" s="7">
-        <v>1</v>
-      </c>
+      <c r="E100" s="7"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="27"/>
+      <c r="A101" s="28"/>
       <c r="B101" s="6"/>
       <c r="C101" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D101" s="6"/>
       <c r="E101" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A102" s="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="28"/>
       <c r="B102" s="6"/>
       <c r="C102" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D102" s="6"/>
       <c r="E102" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="27"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="28"/>
       <c r="B103" s="6"/>
       <c r="C103" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D103" s="6"/>
       <c r="E103" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="27"/>
+      <c r="A104" s="28"/>
       <c r="B104" s="6"/>
       <c r="C104" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D104" s="6"/>
       <c r="E104" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="28"/>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D105" s="6"/>
+      <c r="E105" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A105" s="27"/>
-      <c r="B105" s="6" t="s">
+    <row r="106" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A106" s="28"/>
+      <c r="B106" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6" t="s">
+      <c r="C106" s="6"/>
+      <c r="D106" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E105" s="7"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="27"/>
-      <c r="B106" s="6"/>
-      <c r="C106" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D106" s="6"/>
-      <c r="E106" s="7">
-        <v>1</v>
-      </c>
+      <c r="E106" s="7"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="27"/>
+      <c r="A107" s="28"/>
       <c r="B107" s="6"/>
       <c r="C107" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D107" s="6"/>
       <c r="E107" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="28"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D108" s="6"/>
       <c r="E108" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="27"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="28"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D109" s="6"/>
       <c r="E109" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="27"/>
+      <c r="A110" s="28"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D110" s="6"/>
       <c r="E110" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="28"/>
+      <c r="B111" s="6"/>
+      <c r="C111" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D111" s="6"/>
+      <c r="E111" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A111" s="27"/>
-      <c r="B111" s="6" t="s">
+    <row r="112" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A112" s="28"/>
+      <c r="B112" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C111" s="6"/>
-      <c r="D111" s="6" t="s">
+      <c r="C112" s="6"/>
+      <c r="D112" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E111" s="7"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="27"/>
-      <c r="B112" s="6"/>
-      <c r="C112" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D112" s="6"/>
-      <c r="E112" s="7">
-        <v>1</v>
-      </c>
+      <c r="E112" s="7"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="27"/>
+      <c r="A113" s="28"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D113" s="6"/>
       <c r="E113" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="28"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D114" s="6"/>
       <c r="E114" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="27"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A115" s="28"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D115" s="6"/>
       <c r="E115" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="27"/>
+      <c r="A116" s="28"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D116" s="6"/>
       <c r="E116" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="28"/>
+      <c r="B117" s="6"/>
+      <c r="C117" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D117" s="6"/>
+      <c r="E117" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A117" s="27"/>
-      <c r="B117" s="6" t="s">
+    <row r="118" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A118" s="28"/>
+      <c r="B118" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C117" s="6"/>
-      <c r="D117" s="6" t="s">
+      <c r="C118" s="6"/>
+      <c r="D118" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E117" s="7"/>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="27"/>
-      <c r="B118" s="6"/>
-      <c r="C118" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D118" s="6"/>
-      <c r="E118" s="7">
-        <v>1</v>
-      </c>
+      <c r="E118" s="7"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="27"/>
+      <c r="A119" s="28"/>
       <c r="B119" s="6"/>
       <c r="C119" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D119" s="6"/>
       <c r="E119" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="28"/>
       <c r="B120" s="6"/>
       <c r="C120" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D120" s="6"/>
       <c r="E120" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="27"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="28"/>
       <c r="B121" s="6"/>
       <c r="C121" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D121" s="6"/>
       <c r="E121" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="27"/>
+      <c r="A122" s="28"/>
       <c r="B122" s="6"/>
       <c r="C122" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D122" s="6"/>
       <c r="E122" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="28"/>
+      <c r="B123" s="6"/>
+      <c r="C123" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D123" s="6"/>
+      <c r="E123" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A123" s="27"/>
-      <c r="B123" s="6" t="s">
+    <row r="124" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A124" s="28"/>
+      <c r="B124" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C123" s="6"/>
-      <c r="D123" s="6" t="s">
+      <c r="C124" s="6"/>
+      <c r="D124" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E123" s="7"/>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="27"/>
-      <c r="B124" s="6"/>
-      <c r="C124" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D124" s="6"/>
-      <c r="E124" s="7">
-        <v>1</v>
-      </c>
+      <c r="E124" s="7"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="27"/>
+      <c r="A125" s="28"/>
       <c r="B125" s="6"/>
       <c r="C125" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D125" s="6"/>
       <c r="E125" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A126" s="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="28"/>
       <c r="B126" s="6"/>
       <c r="C126" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D126" s="6"/>
       <c r="E126" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="27"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A127" s="28"/>
       <c r="B127" s="6"/>
       <c r="C127" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D127" s="6"/>
       <c r="E127" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" s="27"/>
+      <c r="A128" s="28"/>
       <c r="B128" s="6"/>
       <c r="C128" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D128" s="6"/>
       <c r="E128" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="28"/>
+      <c r="B129" s="6"/>
+      <c r="C129" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D129" s="6"/>
+      <c r="E129" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="28"/>
-      <c r="B129" s="11"/>
-      <c r="C129" s="11"/>
-      <c r="D129" s="11"/>
-      <c r="E129" s="18"/>
-    </row>
-    <row r="130" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A130" s="13"/>
-      <c r="B130" s="4"/>
-      <c r="C130" s="4"/>
-      <c r="D130" s="4"/>
-      <c r="E130" s="5" t="s">
+    <row r="130" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="29"/>
+      <c r="B130" s="11"/>
+      <c r="C130" s="11"/>
+      <c r="D130" s="11"/>
+      <c r="E130" s="18"/>
+    </row>
+    <row r="131" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A131" s="13"/>
+      <c r="B131" s="4"/>
+      <c r="C131" s="4"/>
+      <c r="D131" s="4"/>
+      <c r="E131" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A131" s="27" t="s">
+    <row r="132" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A132" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="B131" s="6" t="s">
+      <c r="B132" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C131" s="6"/>
-      <c r="D131" s="6" t="s">
+      <c r="C132" s="6"/>
+      <c r="D132" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E131" s="7"/>
-    </row>
-    <row r="132" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A132" s="27"/>
-      <c r="B132" s="6"/>
-      <c r="C132" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D132" s="6"/>
-      <c r="E132" s="7">
-        <v>1</v>
-      </c>
+      <c r="E132" s="7"/>
     </row>
     <row r="133" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A133" s="27"/>
+      <c r="A133" s="28"/>
       <c r="B133" s="6"/>
       <c r="C133" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D133" s="6"/>
       <c r="E133" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A134" s="28"/>
+      <c r="B134" s="6"/>
+      <c r="C134" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D134" s="6"/>
+      <c r="E134" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A134" s="27"/>
-      <c r="B134" s="6" t="s">
+    <row r="135" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A135" s="28"/>
+      <c r="B135" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C134" s="6"/>
-      <c r="D134" s="6" t="s">
+      <c r="C135" s="6"/>
+      <c r="D135" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E134" s="7"/>
-    </row>
-    <row r="135" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A135" s="27"/>
-      <c r="B135" s="6"/>
-      <c r="C135" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D135" s="6"/>
-      <c r="E135" s="7">
-        <v>1</v>
-      </c>
+      <c r="E135" s="7"/>
     </row>
     <row r="136" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A136" s="27"/>
+      <c r="A136" s="28"/>
       <c r="B136" s="6"/>
       <c r="C136" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D136" s="6"/>
       <c r="E136" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A137" s="28"/>
+      <c r="B137" s="6"/>
+      <c r="C137" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D137" s="6"/>
+      <c r="E137" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A137" s="27"/>
-      <c r="B137" s="6" t="s">
+    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A138" s="28"/>
+      <c r="B138" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C137" s="6"/>
-      <c r="D137" s="6" t="s">
+      <c r="C138" s="6"/>
+      <c r="D138" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E137" s="7"/>
-    </row>
-    <row r="138" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A138" s="27"/>
-      <c r="B138" s="6"/>
-      <c r="C138" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D138" s="6"/>
-      <c r="E138" s="7">
-        <v>1</v>
-      </c>
+      <c r="E138" s="7"/>
     </row>
     <row r="139" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A139" s="27"/>
+      <c r="A139" s="28"/>
       <c r="B139" s="6"/>
       <c r="C139" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D139" s="6"/>
       <c r="E139" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A140" s="28"/>
+      <c r="B140" s="6"/>
+      <c r="C140" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D140" s="6"/>
+      <c r="E140" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A140" s="27"/>
-      <c r="B140" s="6" t="s">
+    <row r="141" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A141" s="28"/>
+      <c r="B141" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C140" s="6"/>
-      <c r="D140" s="6" t="s">
+      <c r="C141" s="6"/>
+      <c r="D141" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E140" s="7"/>
-    </row>
-    <row r="141" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A141" s="27"/>
-      <c r="B141" s="6"/>
-      <c r="C141" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D141" s="6"/>
-      <c r="E141" s="7">
-        <v>1</v>
-      </c>
+      <c r="E141" s="7"/>
     </row>
     <row r="142" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A142" s="27"/>
+      <c r="A142" s="28"/>
       <c r="B142" s="6"/>
       <c r="C142" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D142" s="6"/>
       <c r="E142" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A143" s="28"/>
+      <c r="B143" s="6"/>
+      <c r="C143" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D143" s="6"/>
+      <c r="E143" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A143" s="27"/>
-      <c r="B143" s="6" t="s">
+    <row r="144" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A144" s="28"/>
+      <c r="B144" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C143" s="6"/>
-      <c r="D143" s="6" t="s">
+      <c r="C144" s="6"/>
+      <c r="D144" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E143" s="7"/>
-    </row>
-    <row r="144" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A144" s="27"/>
-      <c r="B144" s="6"/>
-      <c r="C144" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D144" s="6"/>
-      <c r="E144" s="7">
-        <v>0</v>
-      </c>
+      <c r="E144" s="7"/>
     </row>
     <row r="145" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A145" s="27"/>
+      <c r="A145" s="28"/>
       <c r="B145" s="6"/>
       <c r="C145" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D145" s="6"/>
       <c r="E145" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A146" s="27"/>
-      <c r="B146" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A146" s="28"/>
+      <c r="B146" s="6"/>
+      <c r="C146" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D146" s="6"/>
+      <c r="E146" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A147" s="28"/>
+      <c r="B147" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C146" s="6"/>
-      <c r="D146" s="6" t="s">
+      <c r="C147" s="6"/>
+      <c r="D147" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E146" s="7"/>
-    </row>
-    <row r="147" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A147" s="27"/>
-      <c r="B147" s="6"/>
-      <c r="C147" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D147" s="6"/>
-      <c r="E147" s="7">
-        <v>0</v>
-      </c>
+      <c r="E147" s="7"/>
     </row>
     <row r="148" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A148" s="27"/>
+      <c r="A148" s="28"/>
       <c r="B148" s="6"/>
       <c r="C148" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D148" s="6"/>
       <c r="E148" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A149" s="27"/>
-      <c r="B149" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A149" s="28"/>
+      <c r="B149" s="6"/>
+      <c r="C149" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D149" s="6"/>
+      <c r="E149" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A150" s="28"/>
+      <c r="B150" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C149" s="6"/>
-      <c r="D149" s="6" t="s">
+      <c r="C150" s="6"/>
+      <c r="D150" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E149" s="7"/>
-    </row>
-    <row r="150" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A150" s="27"/>
-      <c r="B150" s="6"/>
-      <c r="C150" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D150" s="6"/>
-      <c r="E150" s="7">
-        <v>0</v>
-      </c>
+      <c r="E150" s="7"/>
     </row>
     <row r="151" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A151" s="27"/>
+      <c r="A151" s="28"/>
       <c r="B151" s="6"/>
       <c r="C151" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D151" s="6"/>
       <c r="E151" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A152" s="27"/>
-      <c r="B152" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A152" s="28"/>
+      <c r="B152" s="6"/>
+      <c r="C152" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D152" s="6"/>
+      <c r="E152" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A153" s="28"/>
+      <c r="B153" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C152" s="6"/>
-      <c r="D152" s="6" t="s">
+      <c r="C153" s="6"/>
+      <c r="D153" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E152" s="7"/>
-    </row>
-    <row r="153" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A153" s="27"/>
-      <c r="B153" s="6"/>
-      <c r="C153" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D153" s="6"/>
-      <c r="E153" s="7">
-        <v>0</v>
-      </c>
+      <c r="E153" s="7"/>
     </row>
     <row r="154" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A154" s="27"/>
+      <c r="A154" s="28"/>
       <c r="B154" s="6"/>
       <c r="C154" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D154" s="6"/>
       <c r="E154" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A155" s="27"/>
-      <c r="B155" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A155" s="28"/>
+      <c r="B155" s="6"/>
+      <c r="C155" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D155" s="6"/>
+      <c r="E155" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A156" s="28"/>
+      <c r="B156" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C155" s="6"/>
-      <c r="D155" s="6" t="s">
+      <c r="C156" s="6"/>
+      <c r="D156" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="E155" s="7"/>
-    </row>
-    <row r="156" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A156" s="27"/>
-      <c r="B156" s="6"/>
-      <c r="C156" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D156" s="6"/>
-      <c r="E156" s="7">
-        <v>0</v>
-      </c>
+      <c r="E156" s="7"/>
     </row>
     <row r="157" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A157" s="27"/>
+      <c r="A157" s="28"/>
       <c r="B157" s="6"/>
       <c r="C157" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D157" s="6"/>
       <c r="E157" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A158" s="27"/>
-      <c r="B158" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A158" s="28"/>
+      <c r="B158" s="6"/>
+      <c r="C158" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D158" s="6"/>
+      <c r="E158" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A159" s="28"/>
+      <c r="B159" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C158" s="6"/>
-      <c r="D158" s="6" t="s">
+      <c r="C159" s="6"/>
+      <c r="D159" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E158" s="7"/>
-    </row>
-    <row r="159" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A159" s="27"/>
-      <c r="B159" s="6"/>
-      <c r="C159" s="6" t="s">
+      <c r="E159" s="7"/>
+    </row>
+    <row r="160" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A160" s="28"/>
+      <c r="B160" s="6"/>
+      <c r="C160" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D159" s="6"/>
-      <c r="E159" s="7">
+      <c r="D160" s="6"/>
+      <c r="E160" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="28"/>
-      <c r="B160" s="11"/>
-      <c r="C160" s="11" t="s">
+    <row r="161" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="29"/>
+      <c r="B161" s="11"/>
+      <c r="C161" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D160" s="11"/>
-      <c r="E160" s="18">
+      <c r="D161" s="11"/>
+      <c r="E161" s="18">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A69:A129"/>
-    <mergeCell ref="A131:A160"/>
+    <mergeCell ref="A70:A130"/>
+    <mergeCell ref="A132:A161"/>
     <mergeCell ref="A4:A23"/>
     <mergeCell ref="A24:A68"/>
   </mergeCells>

</xml_diff>

<commit_message>
new data, new export
</commit_message>
<xml_diff>
--- a/xp/log_questionnaire_XP_WEEK2_EXPLAINED.xlsx
+++ b/xp/log_questionnaire_XP_WEEK2_EXPLAINED.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Constant\Source\Repos\sorcerer\xp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Source\Repos\sorcerer\xp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="0" windowWidth="27780" windowHeight="12285"/>
+    <workbookView xWindow="5730" yWindow="0" windowWidth="27780" windowHeight="12285"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -377,9 +377,6 @@
     <t>IDjoueur</t>
   </si>
   <si>
-    <t>GLOBAL : transformer toutes les , en _</t>
-  </si>
-  <si>
     <t>profil joueur jeux favoris</t>
   </si>
   <si>
@@ -387,6 +384,9 @@
   </si>
   <si>
     <t>jeuxFav</t>
+  </si>
+  <si>
+    <t>GLOBAL : transformer toutes les , ; et . en _</t>
   </si>
 </sst>
 </file>
@@ -893,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1654,14 +1654,14 @@
     </row>
     <row r="69" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B69" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>119</v>
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E69" s="7"/>
     </row>

</xml_diff>